<commit_message>
Bsp. Datenbank als Excel und erste Einleseversuche
2 Exceldatenbanken mit 50 Einträgen sowie das einlesen als dataframe
</commit_message>
<xml_diff>
--- a/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
+++ b/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jendr\OneDrive\Desktop\Uni\Materialreihenfolge_Stahl_IT_Systeme\MATERIALREIHENFOLGE_STAHL\REIHENFOLGE_APP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenny\Desktop\AO\Master\IT_Projekt\Materialreihenfolge_git\MATERIALREIHENFOLGE_STAHL\REIHENFOLGE_APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4861809C-32EC-4000-9AE0-C69ABAFBC579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF3DBB85-563C-4E4D-AD0D-6098C5D8E0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7AC892B6-DB26-49F7-97F1-210CEAECA503}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{7AC892B6-DB26-49F7-97F1-210CEAECA503}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -398,15 +398,15 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="3" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,654 +417,551 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
-        <f ca="1">RANDBETWEEN(0,1000)</f>
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B51" ca="1" si="0">RANDBETWEEN(0,100)</f>
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C51" ca="1" si="1">RANDBETWEEN(0,1000)</f>
-        <v>246</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>475</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>252</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>638</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>873</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>579</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>789</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>781</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>421</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>299</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>237</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>364</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>187</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>319</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>891</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>298</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>316</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>327</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>880</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>4</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>794</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>326</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>199</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>583</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>891</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>898</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>837</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>332</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>321</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>899</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>754</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>176</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>260</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>995</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>904</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>877</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>258</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>289</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>333</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>151</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>477</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>335</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
-        <v>50</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B51" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>486</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added missing RecordID of Line 50
</commit_message>
<xml_diff>
--- a/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
+++ b/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenny\Desktop\AO\Master\IT_Projekt\Materialreihenfolge_git\MATERIALREIHENFOLGE_STAHL\REIHENFOLGE_APP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jendr\OneDrive\Desktop\Uni\Materialreihenfolge_Stahl_IT_Systeme\MATERIALREIHENFOLGE_STAHL\REIHENFOLGE_APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF3DBB85-563C-4E4D-AD0D-6098C5D8E0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD340DDC-DD16-4CC9-9B87-BF4C4F024309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{7AC892B6-DB26-49F7-97F1-210CEAECA503}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7AC892B6-DB26-49F7-97F1-210CEAECA503}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -397,16 +397,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883430F-FDA4-4C13-80DC-22D4783C8059}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -428,7 +426,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -439,7 +437,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -450,7 +448,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -461,7 +459,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -472,7 +470,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -483,7 +481,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -494,7 +492,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -505,7 +503,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -516,7 +514,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -527,7 +525,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -538,7 +536,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -549,7 +547,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -560,7 +558,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -571,7 +569,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -582,7 +580,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -593,7 +591,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -604,7 +602,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -615,7 +613,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -626,7 +624,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -637,7 +635,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -648,7 +646,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -659,7 +657,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -670,7 +668,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -681,7 +679,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -692,7 +690,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -703,7 +701,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -714,7 +712,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -725,7 +723,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -736,7 +734,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -747,7 +745,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -758,7 +756,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -769,7 +767,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -780,7 +778,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -791,7 +789,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -802,7 +800,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -813,7 +811,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -824,7 +822,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -835,7 +833,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -846,7 +844,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -857,7 +855,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -868,7 +866,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -879,7 +877,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -890,7 +888,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -901,7 +899,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -912,7 +910,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -923,7 +921,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -934,7 +932,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -945,7 +943,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -956,7 +954,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
       <c r="B51" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Included html and js, changed view to right file default 0/0
</commit_message>
<xml_diff>
--- a/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
+++ b/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jendr\OneDrive\Desktop\Uni\Materialreihenfolge_Stahl_IT_Systeme\MATERIALREIHENFOLGE_STAHL\REIHENFOLGE_APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD340DDC-DD16-4CC9-9B87-BF4C4F024309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4861809C-32EC-4000-9AE0-C69ABAFBC579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7AC892B6-DB26-49F7-97F1-210CEAECA503}"/>
   </bookViews>
@@ -397,7 +397,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883430F-FDA4-4C13-80DC-22D4783C8059}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -420,10 +422,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <f ca="1">RANDBETWEEN(0,100)</f>
+        <v>44</v>
       </c>
       <c r="C2" s="1">
-        <v>950</v>
+        <f ca="1">RANDBETWEEN(0,1000)</f>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -431,10 +435,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>5</v>
+        <f t="shared" ref="B3:B51" ca="1" si="0">RANDBETWEEN(0,100)</f>
+        <v>98</v>
       </c>
       <c r="C3" s="1">
-        <v>250</v>
+        <f t="shared" ref="C3:C51" ca="1" si="1">RANDBETWEEN(0,1000)</f>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -442,10 +448,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>750</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -453,10 +461,12 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
       </c>
       <c r="C5" s="1">
-        <v>250</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>475</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -464,10 +474,12 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -475,10 +487,12 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
       </c>
       <c r="C7" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>638</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -486,10 +500,12 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
-        <v>500</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>873</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -497,10 +513,12 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
       </c>
       <c r="C9" s="1">
-        <v>500</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -508,10 +526,12 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
       </c>
       <c r="C10" s="1">
-        <v>700</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>579</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -519,10 +539,12 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
       </c>
       <c r="C11" s="1">
-        <v>800</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>789</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -530,10 +552,12 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
       <c r="C12" s="1">
-        <v>400</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -541,10 +565,12 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
       </c>
       <c r="C13" s="1">
-        <v>700</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>781</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -552,10 +578,12 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
       </c>
       <c r="C14" s="1">
-        <v>450</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -563,10 +591,12 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>850</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -574,10 +604,12 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>53</v>
       </c>
       <c r="C16" s="1">
-        <v>850</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -585,10 +617,12 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="C17" s="1">
-        <v>300</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -596,10 +630,12 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="C18" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -607,10 +643,12 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
       </c>
       <c r="C19" s="1">
-        <v>600</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -618,10 +656,12 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
       </c>
       <c r="C20" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -629,10 +669,12 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
       </c>
       <c r="C21" s="1">
-        <v>900</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -640,10 +682,12 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
       <c r="C22" s="1">
-        <v>300</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>891</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -651,10 +695,12 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
       </c>
       <c r="C23" s="1">
-        <v>350</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -662,10 +708,12 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
       <c r="C24" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -673,10 +721,12 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
       </c>
       <c r="C25" s="1">
-        <v>950</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -684,10 +734,12 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>97</v>
       </c>
       <c r="C26" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>880</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -695,10 +747,12 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>93</v>
       </c>
       <c r="C27" s="1">
-        <v>500</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>794</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -706,10 +760,12 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>997</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -717,10 +773,12 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
       </c>
       <c r="C29" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -728,10 +786,12 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
       </c>
       <c r="C30" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -739,10 +799,12 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
       <c r="C31" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>583</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -750,10 +812,12 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
       <c r="C32" s="1">
-        <v>750</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -761,10 +825,12 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
       </c>
       <c r="C33" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>891</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -772,10 +838,12 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
       </c>
       <c r="C34" s="1">
-        <v>1000</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>898</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -783,10 +851,12 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="C35" s="1">
-        <v>250</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>837</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -794,10 +864,12 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
       </c>
       <c r="C36" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>332</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -805,10 +877,12 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
       <c r="C37" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>321</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -816,10 +890,12 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
       </c>
       <c r="C38" s="1">
-        <v>100</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>899</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -827,10 +903,12 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
       </c>
       <c r="C39" s="1">
-        <v>450</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>754</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -838,10 +916,12 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="C40" s="1">
-        <v>450</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -849,10 +929,12 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
       </c>
       <c r="C41" s="1">
-        <v>400</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -860,10 +942,12 @@
         <v>41</v>
       </c>
       <c r="B42" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
       </c>
       <c r="C42" s="1">
-        <v>800</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>995</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -871,10 +955,12 @@
         <v>42</v>
       </c>
       <c r="B43" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
       </c>
       <c r="C43" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>904</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -882,10 +968,12 @@
         <v>43</v>
       </c>
       <c r="B44" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
       </c>
       <c r="C44" s="1">
-        <v>800</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>877</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -893,10 +981,12 @@
         <v>44</v>
       </c>
       <c r="B45" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
       </c>
       <c r="C45" s="1">
-        <v>950</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -904,10 +994,12 @@
         <v>45</v>
       </c>
       <c r="B46" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
       </c>
       <c r="C46" s="1">
-        <v>1000</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>289</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -915,10 +1007,12 @@
         <v>46</v>
       </c>
       <c r="B47" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
       <c r="C47" s="1">
-        <v>200</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -926,10 +1020,12 @@
         <v>47</v>
       </c>
       <c r="B48" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
       </c>
       <c r="C48" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -937,10 +1033,12 @@
         <v>48</v>
       </c>
       <c r="B49" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
       </c>
       <c r="C49" s="1">
-        <v>700</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>477</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -948,10 +1046,12 @@
         <v>49</v>
       </c>
       <c r="B50" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
       </c>
       <c r="C50" s="1">
-        <v>100</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>335</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -959,10 +1059,12 @@
         <v>50</v>
       </c>
       <c r="B51" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
       </c>
       <c r="C51" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Einbinden von HTML und JS in main project (#4)
* Included html and js, changed view to right file default 0/0

* added script.js

* added storage in var

Co-authored-by: Marcel3197 <mseemann@seetac.de>
</commit_message>
<xml_diff>
--- a/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
+++ b/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jendr\OneDrive\Desktop\Uni\Materialreihenfolge_Stahl_IT_Systeme\MATERIALREIHENFOLGE_STAHL\REIHENFOLGE_APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD340DDC-DD16-4CC9-9B87-BF4C4F024309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4861809C-32EC-4000-9AE0-C69ABAFBC579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7AC892B6-DB26-49F7-97F1-210CEAECA503}"/>
   </bookViews>
@@ -397,7 +397,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883430F-FDA4-4C13-80DC-22D4783C8059}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -420,10 +422,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <f ca="1">RANDBETWEEN(0,100)</f>
+        <v>44</v>
       </c>
       <c r="C2" s="1">
-        <v>950</v>
+        <f ca="1">RANDBETWEEN(0,1000)</f>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -431,10 +435,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>5</v>
+        <f t="shared" ref="B3:B51" ca="1" si="0">RANDBETWEEN(0,100)</f>
+        <v>98</v>
       </c>
       <c r="C3" s="1">
-        <v>250</v>
+        <f t="shared" ref="C3:C51" ca="1" si="1">RANDBETWEEN(0,1000)</f>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -442,10 +448,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>750</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -453,10 +461,12 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
       </c>
       <c r="C5" s="1">
-        <v>250</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>475</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -464,10 +474,12 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -475,10 +487,12 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
       </c>
       <c r="C7" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>638</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -486,10 +500,12 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
-        <v>500</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>873</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -497,10 +513,12 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
       </c>
       <c r="C9" s="1">
-        <v>500</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -508,10 +526,12 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
       </c>
       <c r="C10" s="1">
-        <v>700</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>579</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -519,10 +539,12 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
       </c>
       <c r="C11" s="1">
-        <v>800</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>789</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -530,10 +552,12 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
       <c r="C12" s="1">
-        <v>400</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -541,10 +565,12 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
       </c>
       <c r="C13" s="1">
-        <v>700</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>781</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -552,10 +578,12 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
       </c>
       <c r="C14" s="1">
-        <v>450</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -563,10 +591,12 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>850</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -574,10 +604,12 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>53</v>
       </c>
       <c r="C16" s="1">
-        <v>850</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -585,10 +617,12 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="C17" s="1">
-        <v>300</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -596,10 +630,12 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="C18" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -607,10 +643,12 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
       </c>
       <c r="C19" s="1">
-        <v>600</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -618,10 +656,12 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
       </c>
       <c r="C20" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -629,10 +669,12 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
       </c>
       <c r="C21" s="1">
-        <v>900</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -640,10 +682,12 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
       <c r="C22" s="1">
-        <v>300</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>891</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -651,10 +695,12 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
       </c>
       <c r="C23" s="1">
-        <v>350</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -662,10 +708,12 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
       <c r="C24" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -673,10 +721,12 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
       </c>
       <c r="C25" s="1">
-        <v>950</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -684,10 +734,12 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>97</v>
       </c>
       <c r="C26" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>880</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -695,10 +747,12 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>93</v>
       </c>
       <c r="C27" s="1">
-        <v>500</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>794</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -706,10 +760,12 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>997</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -717,10 +773,12 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
       </c>
       <c r="C29" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -728,10 +786,12 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
       </c>
       <c r="C30" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -739,10 +799,12 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
       <c r="C31" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>583</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -750,10 +812,12 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
       <c r="C32" s="1">
-        <v>750</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -761,10 +825,12 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
       </c>
       <c r="C33" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>891</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -772,10 +838,12 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
       </c>
       <c r="C34" s="1">
-        <v>1000</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>898</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -783,10 +851,12 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="C35" s="1">
-        <v>250</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>837</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -794,10 +864,12 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
       </c>
       <c r="C36" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>332</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -805,10 +877,12 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
       <c r="C37" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>321</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -816,10 +890,12 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
       </c>
       <c r="C38" s="1">
-        <v>100</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>899</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -827,10 +903,12 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
       </c>
       <c r="C39" s="1">
-        <v>450</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>754</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -838,10 +916,12 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="C40" s="1">
-        <v>450</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -849,10 +929,12 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
       </c>
       <c r="C41" s="1">
-        <v>400</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -860,10 +942,12 @@
         <v>41</v>
       </c>
       <c r="B42" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
       </c>
       <c r="C42" s="1">
-        <v>800</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>995</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -871,10 +955,12 @@
         <v>42</v>
       </c>
       <c r="B43" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
       </c>
       <c r="C43" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>904</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -882,10 +968,12 @@
         <v>43</v>
       </c>
       <c r="B44" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
       </c>
       <c r="C44" s="1">
-        <v>800</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>877</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -893,10 +981,12 @@
         <v>44</v>
       </c>
       <c r="B45" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
       </c>
       <c r="C45" s="1">
-        <v>950</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -904,10 +994,12 @@
         <v>45</v>
       </c>
       <c r="B46" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
       </c>
       <c r="C46" s="1">
-        <v>1000</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>289</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -915,10 +1007,12 @@
         <v>46</v>
       </c>
       <c r="B47" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
       <c r="C47" s="1">
-        <v>200</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -926,10 +1020,12 @@
         <v>47</v>
       </c>
       <c r="B48" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
       </c>
       <c r="C48" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -937,10 +1033,12 @@
         <v>48</v>
       </c>
       <c r="B49" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
       </c>
       <c r="C49" s="1">
-        <v>700</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>477</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -948,10 +1046,12 @@
         <v>49</v>
       </c>
       <c r="B50" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
       </c>
       <c r="C50" s="1">
-        <v>100</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>335</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -959,10 +1059,12 @@
         <v>50</v>
       </c>
       <c r="B51" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
       </c>
       <c r="C51" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrieren der Reihenfolge & dummy coil identifikation in den Programmteil der durch HTML anfragen ausgeführt wird kopieren der funktionen in utility.py anpassen der neuen infos an das Notwendige Format für JavaScript
</commit_message>
<xml_diff>
--- a/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
+++ b/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jendr\OneDrive\Desktop\Uni\Materialreihenfolge_Stahl_IT_Systeme\MATERIALREIHENFOLGE_STAHL\REIHENFOLGE_APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4861809C-32EC-4000-9AE0-C69ABAFBC579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979A8D07-17C4-4AD7-9748-3F404A6C05FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7AC892B6-DB26-49F7-97F1-210CEAECA503}"/>
   </bookViews>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883430F-FDA4-4C13-80DC-22D4783C8059}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,12 +422,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>44</v>
+        <f ca="1">RANDBETWEEN(30,100)</f>
+        <v>71</v>
       </c>
       <c r="C2" s="1">
-        <f ca="1">RANDBETWEEN(0,1000)</f>
-        <v>148</v>
+        <f ca="1">RANDBETWEEN(300,1000)</f>
+        <v>585</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -435,12 +435,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B51" ca="1" si="0">RANDBETWEEN(0,100)</f>
-        <v>98</v>
+        <f t="shared" ref="B3:B51" ca="1" si="0">RANDBETWEEN(30,100)</f>
+        <v>67</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C51" ca="1" si="1">RANDBETWEEN(0,1000)</f>
-        <v>246</v>
+        <f t="shared" ref="C3:C51" ca="1" si="1">RANDBETWEEN(300,1000)</f>
+        <v>534</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -449,11 +449,11 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>731</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -462,11 +462,11 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>475</v>
+        <v>698</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -475,11 +475,11 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>252</v>
+        <v>408</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -488,11 +488,11 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>638</v>
+        <v>680</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -501,11 +501,11 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>873</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -514,11 +514,11 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <v>907</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -527,11 +527,11 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>579</v>
+        <v>781</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -540,11 +540,11 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>789</v>
+        <v>566</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -553,11 +553,11 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>147</v>
+        <v>907</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -566,11 +566,11 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>781</v>
+        <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -579,11 +579,11 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>421</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -592,11 +592,11 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>299</v>
+        <v>944</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -605,11 +605,11 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>122</v>
+        <v>802</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -618,11 +618,11 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>237</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -631,11 +631,11 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>364</v>
+        <v>806</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -644,11 +644,11 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>878</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -657,11 +657,11 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>187</v>
+        <v>782</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -670,11 +670,11 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>319</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -683,11 +683,11 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>891</v>
+        <v>863</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -696,11 +696,11 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>298</v>
+        <v>441</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -709,11 +709,11 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>316</v>
+        <v>736</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -722,11 +722,11 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>327</v>
+        <v>843</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -735,11 +735,11 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>880</v>
+        <v>658</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -748,11 +748,11 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>794</v>
+        <v>460</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -761,11 +761,11 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>997</v>
+        <v>599</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -774,11 +774,11 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>326</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -787,11 +787,11 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>199</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -800,11 +800,11 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>583</v>
+        <v>636</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -813,11 +813,11 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>101</v>
+        <v>685</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -826,11 +826,11 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>891</v>
+        <v>781</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -839,11 +839,11 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>898</v>
+        <v>488</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -852,11 +852,11 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>837</v>
+        <v>581</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -865,11 +865,11 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>332</v>
+        <v>836</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -878,11 +878,11 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>321</v>
+        <v>734</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -891,11 +891,11 @@
       </c>
       <c r="B38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>899</v>
+        <v>647</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -904,11 +904,11 @@
       </c>
       <c r="B39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>754</v>
+        <v>728</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -917,11 +917,11 @@
       </c>
       <c r="B40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>176</v>
+        <v>967</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -930,11 +930,11 @@
       </c>
       <c r="B41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>260</v>
+        <v>592</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -943,11 +943,11 @@
       </c>
       <c r="B42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C42" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>995</v>
+        <v>390</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -956,11 +956,11 @@
       </c>
       <c r="B43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="C43" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>904</v>
+        <v>353</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -969,11 +969,11 @@
       </c>
       <c r="B44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="C44" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>877</v>
+        <v>892</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -982,11 +982,11 @@
       </c>
       <c r="B45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C45" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>258</v>
+        <v>895</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -995,11 +995,11 @@
       </c>
       <c r="B46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C46" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>289</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1008,11 +1008,11 @@
       </c>
       <c r="B47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C47" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>333</v>
+        <v>946</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1021,11 +1021,11 @@
       </c>
       <c r="B48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C48" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>151</v>
+        <v>527</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1034,11 +1034,11 @@
       </c>
       <c r="B49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="C49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>477</v>
+        <v>732</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1047,11 +1047,11 @@
       </c>
       <c r="B50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="C50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>335</v>
+        <v>935</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1060,11 +1060,11 @@
       </c>
       <c r="B51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>486</v>
+        <v>851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added alternative for loading data from access database
import pyodbc!
- test MS Access Drivers availability for Python
- created new function: get_coils_from_access_db()
- Checking Database Connection in MS Access
- Selecting Data from MS Access Database

Did not add Database to Git yet, then correct path needs to be inserted, column names and dummy coils need to be added
</commit_message>
<xml_diff>
--- a/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
+++ b/MATERIALREIHENFOLGE_STAHL/REIHENFOLGE_APP/default_database1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jendr\OneDrive\Desktop\Uni\Materialreihenfolge_Stahl_IT_Systeme\MATERIALREIHENFOLGE_STAHL\REIHENFOLGE_APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD340DDC-DD16-4CC9-9B87-BF4C4F024309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4861809C-32EC-4000-9AE0-C69ABAFBC579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7AC892B6-DB26-49F7-97F1-210CEAECA503}"/>
   </bookViews>
@@ -397,7 +397,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4883430F-FDA4-4C13-80DC-22D4783C8059}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -420,10 +422,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <f ca="1">RANDBETWEEN(0,100)</f>
+        <v>44</v>
       </c>
       <c r="C2" s="1">
-        <v>950</v>
+        <f ca="1">RANDBETWEEN(0,1000)</f>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -431,10 +435,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>5</v>
+        <f t="shared" ref="B3:B51" ca="1" si="0">RANDBETWEEN(0,100)</f>
+        <v>98</v>
       </c>
       <c r="C3" s="1">
-        <v>250</v>
+        <f t="shared" ref="C3:C51" ca="1" si="1">RANDBETWEEN(0,1000)</f>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -442,10 +448,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>750</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -453,10 +461,12 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>48</v>
       </c>
       <c r="C5" s="1">
-        <v>250</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>475</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -464,10 +474,12 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -475,10 +487,12 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
       </c>
       <c r="C7" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>638</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -486,10 +500,12 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
-        <v>500</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>873</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -497,10 +513,12 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
       </c>
       <c r="C9" s="1">
-        <v>500</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -508,10 +526,12 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
       </c>
       <c r="C10" s="1">
-        <v>700</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>579</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -519,10 +539,12 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
       </c>
       <c r="C11" s="1">
-        <v>800</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>789</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -530,10 +552,12 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
       <c r="C12" s="1">
-        <v>400</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -541,10 +565,12 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
       </c>
       <c r="C13" s="1">
-        <v>700</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>781</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -552,10 +578,12 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
       </c>
       <c r="C14" s="1">
-        <v>450</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -563,10 +591,12 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>850</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -574,10 +604,12 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>53</v>
       </c>
       <c r="C16" s="1">
-        <v>850</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -585,10 +617,12 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="C17" s="1">
-        <v>300</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -596,10 +630,12 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
       <c r="C18" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -607,10 +643,12 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
       </c>
       <c r="C19" s="1">
-        <v>600</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -618,10 +656,12 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
       </c>
       <c r="C20" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -629,10 +669,12 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
       </c>
       <c r="C21" s="1">
-        <v>900</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -640,10 +682,12 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
       </c>
       <c r="C22" s="1">
-        <v>300</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>891</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -651,10 +695,12 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
       </c>
       <c r="C23" s="1">
-        <v>350</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -662,10 +708,12 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
       <c r="C24" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -673,10 +721,12 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
       </c>
       <c r="C25" s="1">
-        <v>950</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -684,10 +734,12 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>97</v>
       </c>
       <c r="C26" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>880</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -695,10 +747,12 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>93</v>
       </c>
       <c r="C27" s="1">
-        <v>500</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>794</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -706,10 +760,12 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>997</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -717,10 +773,12 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
       </c>
       <c r="C29" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -728,10 +786,12 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
       </c>
       <c r="C30" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -739,10 +799,12 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
       <c r="C31" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>583</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -750,10 +812,12 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
       <c r="C32" s="1">
-        <v>750</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -761,10 +825,12 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
       </c>
       <c r="C33" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>891</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -772,10 +838,12 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
       </c>
       <c r="C34" s="1">
-        <v>1000</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>898</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -783,10 +851,12 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="C35" s="1">
-        <v>250</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>837</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -794,10 +864,12 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
       </c>
       <c r="C36" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>332</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -805,10 +877,12 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
       <c r="C37" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>321</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -816,10 +890,12 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
       </c>
       <c r="C38" s="1">
-        <v>100</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>899</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -827,10 +903,12 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
       </c>
       <c r="C39" s="1">
-        <v>450</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>754</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -838,10 +916,12 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="C40" s="1">
-        <v>450</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -849,10 +929,12 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
       </c>
       <c r="C41" s="1">
-        <v>400</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>260</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -860,10 +942,12 @@
         <v>41</v>
       </c>
       <c r="B42" s="1">
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
       </c>
       <c r="C42" s="1">
-        <v>800</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>995</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -871,10 +955,12 @@
         <v>42</v>
       </c>
       <c r="B43" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
       </c>
       <c r="C43" s="1">
-        <v>650</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>904</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -882,10 +968,12 @@
         <v>43</v>
       </c>
       <c r="B44" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
       </c>
       <c r="C44" s="1">
-        <v>800</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>877</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -893,10 +981,12 @@
         <v>44</v>
       </c>
       <c r="B45" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
       </c>
       <c r="C45" s="1">
-        <v>950</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -904,10 +994,12 @@
         <v>45</v>
       </c>
       <c r="B46" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
       </c>
       <c r="C46" s="1">
-        <v>1000</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>289</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -915,10 +1007,12 @@
         <v>46</v>
       </c>
       <c r="B47" s="1">
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
       <c r="C47" s="1">
-        <v>200</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>333</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -926,10 +1020,12 @@
         <v>47</v>
       </c>
       <c r="B48" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
       </c>
       <c r="C48" s="1">
-        <v>150</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -937,10 +1033,12 @@
         <v>48</v>
       </c>
       <c r="B49" s="1">
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
       </c>
       <c r="C49" s="1">
-        <v>700</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>477</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -948,10 +1046,12 @@
         <v>49</v>
       </c>
       <c r="B50" s="1">
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
       </c>
       <c r="C50" s="1">
-        <v>100</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>335</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -959,10 +1059,12 @@
         <v>50</v>
       </c>
       <c r="B51" s="1">
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
       </c>
       <c r="C51" s="1">
-        <v>550</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>